<commit_message>
feature engineering on klasifikasi bertahap
</commit_message>
<xml_diff>
--- a/ProDS2/Prediction/iterasi1.xlsx
+++ b/ProDS2/Prediction/iterasi1.xlsx
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>tank</t>
         </is>
       </c>
     </row>
@@ -777,7 +777,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>settlement</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>settlement</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>forest</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>forest</t>
+          <t>tank</t>
         </is>
       </c>
     </row>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>tank</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -1605,7 +1605,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>agriculture</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -1665,7 +1665,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -1761,7 +1761,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>settlement</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -1893,7 +1893,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -1953,7 +1953,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>agriculture</t>
+          <t>grassland</t>
         </is>
       </c>
     </row>
@@ -2073,7 +2073,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>forest</t>
         </is>
       </c>
     </row>
@@ -2121,7 +2121,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -2217,7 +2217,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>forest</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>agriculture</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -2349,7 +2349,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -2445,7 +2445,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>forest</t>
         </is>
       </c>
     </row>
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -2901,7 +2901,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>settlement</t>
         </is>
       </c>
     </row>
@@ -2913,7 +2913,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>settlement</t>
         </is>
       </c>
     </row>
@@ -2925,7 +2925,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>forest</t>
         </is>
       </c>
     </row>
@@ -2949,7 +2949,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>tank</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>forest</t>
         </is>
       </c>
     </row>
@@ -3105,7 +3105,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -3129,7 +3129,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -3141,7 +3141,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -3165,7 +3165,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>forest</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -3189,7 +3189,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>tank</t>
         </is>
       </c>
     </row>
@@ -3201,7 +3201,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>tank</t>
         </is>
       </c>
     </row>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>tank</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -3393,7 +3393,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -3429,7 +3429,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>settlement</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -3441,7 +3441,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -3645,7 +3645,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>tank</t>
         </is>
       </c>
     </row>
@@ -3705,7 +3705,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -3717,7 +3717,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>agriculture</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -3753,7 +3753,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>tank</t>
         </is>
       </c>
     </row>
@@ -3765,7 +3765,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>tank</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -3777,7 +3777,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -3957,7 +3957,7 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>agriculture</t>
+          <t>grassland</t>
         </is>
       </c>
     </row>
@@ -4077,7 +4077,7 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>settlement</t>
         </is>
       </c>
     </row>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>forest</t>
         </is>
       </c>
     </row>
@@ -4245,7 +4245,7 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>tank</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -4293,7 +4293,7 @@
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -4425,7 +4425,7 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>settlement</t>
         </is>
       </c>
     </row>
@@ -4449,7 +4449,7 @@
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>settlement</t>
         </is>
       </c>
     </row>
@@ -4593,7 +4593,7 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>tank</t>
         </is>
       </c>
     </row>
@@ -4701,7 +4701,7 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -4713,7 +4713,7 @@
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -4893,7 +4893,7 @@
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>forest</t>
+          <t>tank</t>
         </is>
       </c>
     </row>
@@ -5025,7 +5025,7 @@
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>agriculture</t>
+          <t>grassland</t>
         </is>
       </c>
     </row>
@@ -5145,7 +5145,7 @@
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -5205,7 +5205,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>land_without_scrub</t>
         </is>
       </c>
     </row>
@@ -5241,7 +5241,7 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>tank</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -5349,7 +5349,7 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>tank</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -5397,7 +5397,7 @@
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -5433,7 +5433,7 @@
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>agriculture</t>
+          <t>grassland</t>
         </is>
       </c>
     </row>
@@ -5445,7 +5445,7 @@
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>grassland</t>
         </is>
       </c>
     </row>
@@ -5481,7 +5481,7 @@
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -5505,7 +5505,7 @@
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>settlement</t>
+          <t>grassland</t>
         </is>
       </c>
     </row>
@@ -5541,7 +5541,7 @@
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>tank</t>
         </is>
       </c>
     </row>
@@ -5553,7 +5553,7 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>agriculture</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -5565,7 +5565,7 @@
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>land_without_scrub</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>road_n_railway</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -5697,7 +5697,7 @@
       </c>
       <c r="B439" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>river</t>
         </is>
       </c>
     </row>
@@ -5841,7 +5841,7 @@
       </c>
       <c r="B451" t="inlineStr">
         <is>
-          <t>crop</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -5889,7 +5889,7 @@
       </c>
       <c r="B455" t="inlineStr">
         <is>
-          <t>grassland</t>
+          <t>settlement</t>
         </is>
       </c>
     </row>
@@ -5937,7 +5937,7 @@
       </c>
       <c r="B459" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -5949,7 +5949,7 @@
       </c>
       <c r="B460" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>forest</t>
         </is>
       </c>
     </row>
@@ -5973,7 +5973,7 @@
       </c>
       <c r="B462" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -6033,7 +6033,7 @@
       </c>
       <c r="B467" t="inlineStr">
         <is>
-          <t>agriculture</t>
+          <t>crop</t>
         </is>
       </c>
     </row>
@@ -6117,7 +6117,7 @@
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>agriculture</t>
         </is>
       </c>
     </row>
@@ -6129,7 +6129,7 @@
       </c>
       <c r="B475" t="inlineStr">
         <is>
-          <t>tank</t>
+          <t>road_n_railway</t>
         </is>
       </c>
     </row>
@@ -6477,7 +6477,7 @@
       </c>
       <c r="B504" t="inlineStr">
         <is>
-          <t>river</t>
+          <t>tank</t>
         </is>
       </c>
     </row>

</xml_diff>